<commit_message>
added quantity and appended orders to inventory instead
</commit_message>
<xml_diff>
--- a/Assignment 2/orders.xlsx
+++ b/Assignment 2/orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\BCIT Work Synced Folder\My Courses\COMP3522 OOP 2\Winter 2020\Assignments\Assignment 2 Supply Chain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73D80D25-3399-4B0A-ACAB-4530E224E90C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F959E200-ABA9-4C24-84DC-7F0EB85250A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +968,7 @@
         <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S7" t="s">
         <v>34</v>
@@ -1072,6 +1072,12 @@
       <c r="Q10" t="s">
         <v>90</v>
       </c>
+      <c r="R10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1098,12 +1104,6 @@
       <c r="Q11" t="s">
         <v>82</v>
       </c>
-      <c r="R11" t="s">
-        <v>34</v>
-      </c>
-      <c r="S11" t="s">
-        <v>33</v>
-      </c>
       <c r="V11" t="s">
         <v>79</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>89</v>
       </c>
       <c r="R14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S14" t="s">
         <v>33</v>
@@ -1251,7 +1251,7 @@
         <v>77</v>
       </c>
       <c r="R15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S15" t="s">
         <v>34</v>

</xml_diff>